<commit_message>
debug in control code
</commit_message>
<xml_diff>
--- a/控制信号设计.xlsx
+++ b/控制信号设计.xlsx
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="321">
   <si>
     <t>000</t>
   </si>
@@ -458,7 +458,87 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>EQZ</t>
+    <t>0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Branch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BNEZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>funct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>op（15-11）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>立即数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -466,43 +546,658 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>BEQZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>BNEZ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>00010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>—</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>—</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTEQZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUBU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01（1-0）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11（1-0）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>—</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLTU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRLV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01100(4-0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01010(4-0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000(4-0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01101(4-0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00(1-0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00011(4-0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11(1-0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00110(4-0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MFIH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MFPC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTIH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTSP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000000(7-0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01000000(7-0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000001(7-0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDIU3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDIU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDSP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMPI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LW_SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW_RS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW_SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000000（7-0）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>—</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000（10-8）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100（10-8）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011（10-8）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010（10-8）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reg1_select</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reg2_select</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegWrite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>写回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUTB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(钟鸣远校对)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extend(3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reg1_select(3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegWrite（1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jump（1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 No</t>
+  </si>
+  <si>
+    <t>0 No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALUSrc（1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALUOp（4）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegDst（3）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemRead（1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemWrite（1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Branch（3）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemToReg（1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">000 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>0000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 No PC</t>
+  </si>
+  <si>
+    <t>0 No PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 No PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 Write</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 Read</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 ALU</t>
+  </si>
+  <si>
+    <t>1 ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1010 CMPU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>0001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1000</t>
+    <t>0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -510,7 +1205,224 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1010</t>
+    <t>0 Reg</t>
+  </si>
+  <si>
+    <t>0 Reg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 Reg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010 rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 imm</t>
+  </si>
+  <si>
+    <t>1 imm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010 rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101 IH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 imm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 imm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 SP</t>
+  </si>
+  <si>
+    <t>100 SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 RA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLTU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUTA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BEQZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTEQZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reg2_select(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011 T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111 PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">00 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01 rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01 rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01 rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01 rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1100</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -518,403 +1430,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Branch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BEQZ/BTEQZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BNEZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>指令</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>funct</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>op（15-11）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>立即数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NOP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BEQZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BNEZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>—</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>—</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7-0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOVE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7-0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7-0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7-0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10-0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BTEQZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADDU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SUBU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01（1-0）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11（1-0）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>—</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AND</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLTU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SRA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SRLV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01100(4-0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01010(4-0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00000(4-0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01101(4-0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00(1-0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00011(4-0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11(1-0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00110(4-0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MFIH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MFPC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MTIH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MTSP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00000000(7-0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01000000(7-0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00000001(7-0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADDIU3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADDIU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADDSP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMPI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LW_SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SW_RS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SW_SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3-0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4-0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4-0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7-0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7-0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00000000（7-0）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>—</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000（10-8）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100（10-8）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011（10-8）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010（10-8）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMPU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reg1_select</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rs</t>
+    <t>1011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -922,554 +1450,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reg2_select</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RegWrite</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>写回</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OUTPUTA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OUTPUTB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>（钟鸣远校对）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(钟鸣远校对)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>（如何在ID阶段跳转）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Extend(3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reg1_select(3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reg2_select(1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RegWrite（1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jump（1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 No</t>
-  </si>
-  <si>
-    <t>0 No</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALUSrc（1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALUOp（4）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RegDst（3）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemRead（1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemWrite（1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Branch（3）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemToReg（1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">000 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">0 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 No</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>怎么处理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 rt</t>
-  </si>
-  <si>
-    <t>1 rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 No</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 Yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 No PC</t>
-  </si>
-  <si>
-    <t>0 No PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 No PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 Mem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 Write</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 Read</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 ALU</t>
-  </si>
-  <si>
-    <t>1 ALU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 ALU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1010 CMPU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 Reg</t>
-  </si>
-  <si>
-    <t>0 Reg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 Reg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010 rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 imm</t>
-  </si>
-  <si>
-    <t>1 imm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010 rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101 IH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 imm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 imm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100 SP</t>
-  </si>
-  <si>
-    <t>100 SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100 SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100 SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110 PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110 PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110 PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10 RA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 rs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1630,10 +1615,10 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1943,7 +1928,7 @@
   <dimension ref="A1:AV245"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1956,25 +1941,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="18"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="17"/>
+      <c r="E1" s="18"/>
       <c r="F1" s="5"/>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
       <c r="I1" s="5"/>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="17"/>
+      <c r="K1" s="18"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
@@ -2233,9 +2218,7 @@
       <c r="D6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>217</v>
-      </c>
+      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="6" t="s">
         <v>24</v>
@@ -2293,7 +2276,7 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>58</v>
@@ -2359,7 +2342,7 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>59</v>
@@ -2480,7 +2463,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -2526,19 +2509,19 @@
     </row>
     <row r="11" spans="1:48" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>220</v>
+        <v>1</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -2549,59 +2532,56 @@
         <v>39</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>221</v>
+        <v>2</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>86</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>62</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>222</v>
+        <v>3</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>63</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>223</v>
+        <v>294</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>219</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:48" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -2612,21 +2592,27 @@
         <v>50</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="G15" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="16" spans="1:48" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>65</v>
@@ -2637,10 +2623,10 @@
         <v>47</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>66</v>
@@ -2648,27 +2634,27 @@
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>67</v>
@@ -2676,7 +2662,7 @@
     </row>
     <row r="20" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D20" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>68</v>
@@ -2684,65 +2670,52 @@
     </row>
     <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>180</v>
+        <v>291</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>69</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D24" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="25" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>41</v>
@@ -2750,16 +2723,16 @@
     </row>
     <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -2796,10 +2769,10 @@
     </row>
     <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="D32" s="4" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:48" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -2815,10 +2788,10 @@
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -2869,7 +2842,7 @@
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>48</v>
@@ -13426,9 +13399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J32" sqref="J32"/>
+      <selection pane="topRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -13445,78 +13418,78 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>242</v>
+      <c r="E1" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>244</v>
+        <v>303</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="I2" s="3">
         <v>0</v>
@@ -13525,53 +13498,51 @@
         <v>0</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="Q2" s="7"/>
       <c r="R2" s="3"/>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E3" s="2">
         <v>110</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>320</v>
-      </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="8" t="s">
-        <v>244</v>
+        <v>303</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -13579,1188 +13550,1184 @@
         <v>52</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>249</v>
+        <v>8</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="3"/>
     </row>
     <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E4" s="2">
         <v>100</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>321</v>
+        <v>299</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>199</v>
+        <v>304</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>264</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
         <v>52</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="O4" s="3"/>
+        <v>232</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>316</v>
+      </c>
       <c r="P4" s="3" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="Q4" s="7"/>
       <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="D5" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E5" s="2">
         <v>100</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>199</v>
+        <v>304</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
-        <v>179</v>
-      </c>
+      <c r="K5" s="3"/>
       <c r="L5" s="3" t="s">
         <v>52</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="O5" s="3"/>
+        <v>218</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>317</v>
+      </c>
       <c r="P5" s="3" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="Q5" s="7"/>
       <c r="R5" s="3"/>
     </row>
     <row r="6" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E6" s="2">
         <v>100</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>199</v>
+        <v>305</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
-        <v>273</v>
-      </c>
+      <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
         <v>52</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>267</v>
+        <v>318</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="Q6" s="7"/>
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>115</v>
-      </c>
       <c r="D7" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>52</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>252</v>
+        <v>306</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>52</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="3"/>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>116</v>
-      </c>
       <c r="D8" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>254</v>
+        <v>307</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>285</v>
+        <v>259</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>38</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="Q8" s="7"/>
       <c r="R8" s="3"/>
     </row>
     <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>254</v>
+        <v>308</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q9" s="7"/>
       <c r="R9" s="3"/>
     </row>
     <row r="10" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>251</v>
+        <v>307</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>294</v>
+        <v>268</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q10" s="7"/>
       <c r="R10" s="3"/>
     </row>
     <row r="11" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>251</v>
+        <v>307</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>275</v>
+        <v>312</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q11" s="7"/>
       <c r="R11" s="3"/>
     </row>
     <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>296</v>
+        <v>270</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>251</v>
+        <v>307</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q12" s="7"/>
       <c r="R12" s="3"/>
     </row>
     <row r="13" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>38</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>297</v>
+        <v>271</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>298</v>
+        <v>272</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q13" s="7"/>
       <c r="R13" s="3"/>
     </row>
     <row r="14" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>52</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="G14" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>276</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>46</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q14" s="7"/>
       <c r="R14" s="3"/>
     </row>
     <row r="15" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>297</v>
+        <v>271</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q15" s="7"/>
       <c r="R15" s="3"/>
     </row>
     <row r="16" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>302</v>
+        <v>276</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>304</v>
+        <v>277</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>37</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q16" s="7"/>
       <c r="R16" s="3"/>
     </row>
     <row r="17" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>142</v>
-      </c>
       <c r="C17" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>52</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>298</v>
+        <v>272</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>199</v>
+        <v>319</v>
       </c>
       <c r="Q17" s="7"/>
       <c r="R17" s="3"/>
     </row>
     <row r="18" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>143</v>
-      </c>
       <c r="C18" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>199</v>
+        <v>17</v>
       </c>
       <c r="Q18" s="7"/>
       <c r="R18" s="3"/>
     </row>
     <row r="19" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>144</v>
-      </c>
       <c r="C19" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
-        <v>307</v>
+        <v>280</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>311</v>
+        <v>281</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>199</v>
+        <v>320</v>
       </c>
       <c r="Q19" s="7"/>
       <c r="R19" s="3"/>
     </row>
     <row r="20" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3" t="s">
-        <v>181</v>
+        <v>80</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>47</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>199</v>
+        <v>17</v>
       </c>
       <c r="Q20" s="7"/>
       <c r="R20" s="3"/>
     </row>
     <row r="21" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>313</v>
+        <v>283</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>312</v>
+        <v>282</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>37</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O21" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q21" s="7"/>
       <c r="R21" s="3"/>
     </row>
     <row r="22" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O22" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="Q22" s="7"/>
       <c r="R22" s="3"/>
     </row>
     <row r="23" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="14" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>252</v>
+        <v>310</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>314</v>
+        <v>284</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="O23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="Q23" s="7"/>
       <c r="R23" s="3"/>
     </row>
     <row r="24" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>313</v>
+        <v>283</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O24" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q24" s="7"/>
       <c r="R24" s="3"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>46</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>316</v>
+        <v>286</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O25" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q25" s="7"/>
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3" t="s">
-        <v>317</v>
+        <v>287</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>46</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O26" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q26" s="7"/>
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>47</v>
@@ -14768,227 +14735,225 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
-        <v>298</v>
+        <v>272</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>282</v>
+        <v>312</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O27" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="Q27" s="7"/>
       <c r="R27" s="1"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>318</v>
+        <v>288</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O28" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="Q28" s="7"/>
       <c r="R28" s="1"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="15" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>178</v>
-      </c>
       <c r="D29" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>319</v>
+        <v>289</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>323</v>
+        <v>290</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="O29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="Q29" s="7"/>
       <c r="R29" s="1"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="15" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>46</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>315</v>
+        <v>285</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="Q30" s="7"/>
       <c r="R30" s="1"/>
     </row>
     <row r="31" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A31" s="16" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>231</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="L31" s="3"/>
       <c r="M31" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="O31" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="Q31" s="7"/>
       <c r="R31" s="3"/>

</xml_diff>

<commit_message>
delete pre files and update some new files
</commit_message>
<xml_diff>
--- a/控制信号设计.xlsx
+++ b/控制信号设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="单个控制信号" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="329">
   <si>
     <t>000</t>
   </si>
@@ -956,6 +956,18 @@
     <t>0</t>
   </si>
   <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegWrite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -964,15 +976,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RegWrite</t>
+    <t>写回</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -984,7 +988,106 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>写回</t>
+    <t>OUTPUTB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(钟鸣远校对)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extend(3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reg1_select(3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegWrite（1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jump（1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 No</t>
+  </si>
+  <si>
+    <t>0 No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALUSrc（1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALUOp（4）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegDst（3）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemRead（1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemWrite（1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Branch（3）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemToReg（1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">000 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -992,11 +1095,254 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 No PC</t>
+  </si>
+  <si>
+    <t>0 No PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 No PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OUTPUTB</t>
+    <t>1 Write</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 Read</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 ALU</t>
+  </si>
+  <si>
+    <t>1 ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1010 CMPU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 Reg</t>
+  </si>
+  <si>
+    <t>0 Reg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 Reg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010 rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 imm</t>
+  </si>
+  <si>
+    <t>1 imm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010 rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101 IH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 imm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 imm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 SP</t>
+  </si>
+  <si>
+    <t>100 SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLTU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUTA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BEQZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTEQZ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1004,23 +1350,75 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(钟鸣远校对)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reg2_select(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001 rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011 T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111 PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">00 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01 rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01 rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01 rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01 rt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1028,121 +1426,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Extend(3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reg1_select(3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RegWrite（1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jump（1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 No</t>
-  </si>
-  <si>
-    <t>0 No</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALUSrc（1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALUOp（4）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RegDst（3）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemRead（1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemWrite（1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Branch（3）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemToReg（1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">000 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">0 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 No</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 No</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 Yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 No PC</t>
-  </si>
-  <si>
-    <t>0 No PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 No PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
+    <t>011</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1150,243 +1434,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1 Write</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 Read</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 ALU</t>
-  </si>
-  <si>
-    <t>1 ALU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 ALU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1010 CMPU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 Reg</t>
-  </si>
-  <si>
-    <t>0 Reg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0 Reg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010 rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 imm</t>
-  </si>
-  <si>
-    <t>1 imm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010 rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101 IH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 imm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 imm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100 SP</t>
-  </si>
-  <si>
-    <t>100 SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100 SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100 SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10 RA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLTU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OUTPUTA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BEQZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BTEQZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reg2_select(2)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011 T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111 PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">00 </t>
+    <t>10 rs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1398,63 +1450,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>01 rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01 rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01 rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01 rt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
+    <t>00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11 RA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1927,8 +1959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV245"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2276,7 +2308,7 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>58</v>
@@ -2342,7 +2374,7 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>59</v>
@@ -2541,7 +2573,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -2578,10 +2610,10 @@
         <v>63</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:48" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -2598,10 +2630,10 @@
         <v>64</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:48" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -2676,66 +2708,72 @@
         <v>79</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>194</v>
+        <v>323</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>196</v>
+        <v>324</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>197</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>175</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
     <row r="25" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
+      <c r="A25" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>201</v>
+      <c r="A27" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="D28" s="4" t="s">
         <v>52</v>
       </c>
@@ -2744,6 +2782,12 @@
       </c>
     </row>
     <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>199</v>
+      </c>
       <c r="D29" s="4" t="s">
         <v>53</v>
       </c>
@@ -2769,10 +2813,10 @@
     </row>
     <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="D32" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:48" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -2791,7 +2835,7 @@
         <v>181</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -2842,7 +2886,7 @@
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>48</v>
@@ -13399,9 +13443,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G19" sqref="G19"/>
+      <selection pane="topRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -13430,40 +13474,40 @@
         <v>88</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="G1" s="17" t="s">
-        <v>298</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>217</v>
-      </c>
       <c r="J1" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="O1" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="P1" s="17" t="s">
         <v>224</v>
-      </c>
-      <c r="O1" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="P1" s="17" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -13480,16 +13524,16 @@
         <v>96</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I2" s="3">
         <v>0</v>
@@ -13498,22 +13542,22 @@
         <v>0</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="Q2" s="7"/>
       <c r="R2" s="3"/>
@@ -13536,13 +13580,13 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -13550,16 +13594,16 @@
         <v>52</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="3"/>
@@ -13581,16 +13625,16 @@
         <v>100</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -13598,16 +13642,16 @@
         <v>52</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="Q4" s="7"/>
       <c r="R4" s="3"/>
@@ -13629,16 +13673,16 @@
         <v>100</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -13646,16 +13690,16 @@
         <v>52</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Q5" s="7"/>
       <c r="R5" s="3"/>
@@ -13677,16 +13721,16 @@
         <v>100</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -13694,13 +13738,13 @@
         <v>52</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>193</v>
@@ -13725,19 +13769,19 @@
         <v>52</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>70</v>
@@ -13746,16 +13790,16 @@
         <v>38</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>52</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="3"/>
@@ -13774,22 +13818,22 @@
         <v>113</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>71</v>
@@ -13798,16 +13842,16 @@
         <v>38</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="Q8" s="7"/>
       <c r="R8" s="3"/>
@@ -13829,37 +13873,37 @@
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>72</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q9" s="7"/>
       <c r="R9" s="3"/>
@@ -13881,37 +13925,37 @@
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>180</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q10" s="7"/>
       <c r="R10" s="3"/>
@@ -13933,37 +13977,37 @@
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G11" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="K11" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>312</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q11" s="7"/>
       <c r="R11" s="3"/>
@@ -13985,37 +14029,37 @@
         <v>0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>73</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q12" s="7"/>
       <c r="R12" s="3"/>
@@ -14037,17 +14081,19 @@
         <v>38</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="G13" s="3"/>
+        <v>269</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="H13" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>75</v>
@@ -14056,16 +14102,16 @@
         <v>40</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q13" s="7"/>
       <c r="R13" s="3"/>
@@ -14087,37 +14133,37 @@
         <v>52</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>46</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q14" s="7"/>
       <c r="R14" s="3"/>
@@ -14139,35 +14185,37 @@
         <v>178</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="G15" s="3"/>
+        <v>269</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="H15" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q15" s="7"/>
       <c r="R15" s="3"/>
@@ -14186,22 +14234,22 @@
         <v>113</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>76</v>
@@ -14210,16 +14258,16 @@
         <v>37</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q16" s="7"/>
       <c r="R16" s="3"/>
@@ -14241,33 +14289,35 @@
         <v>52</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="G17" s="3"/>
+        <v>276</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="H17" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="Q17" s="7"/>
       <c r="R17" s="3"/>
@@ -14289,27 +14339,29 @@
         <v>0</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="G18" s="3"/>
+        <v>299</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>317</v>
+      </c>
       <c r="H18" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>0</v>
@@ -14337,33 +14389,35 @@
         <v>0</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="G19" s="3"/>
+        <v>232</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>318</v>
+      </c>
       <c r="H19" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="Q19" s="7"/>
       <c r="R19" s="3"/>
@@ -14385,14 +14439,16 @@
         <v>0</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="G20" s="3"/>
+        <v>232</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>319</v>
+      </c>
       <c r="H20" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3" t="s">
@@ -14402,10 +14458,10 @@
         <v>47</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O20" s="3" t="s">
         <v>0</v>
@@ -14433,35 +14489,37 @@
         <v>40</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="G21" s="3"/>
+        <v>281</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>320</v>
+      </c>
       <c r="H21" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>37</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O21" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q21" s="7"/>
       <c r="R21" s="3"/>
@@ -14483,29 +14541,31 @@
         <v>37</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="G22" s="3"/>
+        <v>232</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="H22" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>70</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O22" s="3" t="s">
         <v>0</v>
@@ -14530,32 +14590,32 @@
         <v>160</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O23" s="3" t="s">
         <v>0</v>
@@ -14583,35 +14643,37 @@
         <v>180</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="G24" s="3"/>
+        <v>281</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="H24" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O24" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q24" s="7"/>
       <c r="R24" s="3"/>
@@ -14633,35 +14695,37 @@
         <v>46</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="G25" s="3"/>
+        <v>284</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="H25" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>70</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O25" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q25" s="7"/>
       <c r="R25" s="1"/>
@@ -14683,35 +14747,37 @@
         <v>179</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="G26" s="3"/>
+        <v>231</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="H26" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>46</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O26" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q26" s="7"/>
       <c r="R26" s="1"/>
@@ -14733,33 +14799,35 @@
         <v>47</v>
       </c>
       <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="H27" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O27" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q27" s="7"/>
       <c r="R27" s="1"/>
@@ -14781,29 +14849,31 @@
         <v>180</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="G28" s="3"/>
+        <v>286</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>321</v>
+      </c>
       <c r="H28" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>70</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O28" s="3" t="s">
         <v>0</v>
@@ -14828,32 +14898,32 @@
         <v>103</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>290</v>
+        <v>322</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>70</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O29" s="3" t="s">
         <v>0</v>
@@ -14881,29 +14951,29 @@
         <v>46</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>70</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>0</v>
@@ -14928,15 +14998,17 @@
         <v>169</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="G31" s="3"/>
+        <v>231</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3" t="s">
@@ -14944,10 +15016,10 @@
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O31" s="3" t="s">
         <v>0</v>
@@ -15051,6 +15123,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor modifications in port
</commit_message>
<xml_diff>
--- a/控制信号设计.xlsx
+++ b/控制信号设计.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28908"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jason/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="11200" yWindow="5860" windowWidth="28800" windowHeight="17540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="单个控制信号" sheetId="1" r:id="rId1"/>
     <sheet name="控制信号流程" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>作者</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="J2" authorId="0" shapeId="0">
+    <comment ref="J2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -31,7 +44,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -46,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0">
+    <comment ref="G10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +70,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -79,10 +92,10 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>作者</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment ref="A3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +106,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -108,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +132,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -134,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0" shapeId="0">
+    <comment ref="A21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -145,7 +158,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -160,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A31" authorId="0" shapeId="0">
+    <comment ref="A31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -171,7 +184,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:
+          <t>Author:
 J型</t>
         </r>
       </text>
@@ -181,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="319">
   <si>
     <t>000</t>
   </si>
@@ -734,10 +747,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>11101</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1334,10 +1343,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>10 RA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SLTU</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1382,14 +1387,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>111 PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">00 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1410,18 +1407,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>00 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>01 rt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>00 rs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1100</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1456,6 +1445,18 @@
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 rs</t>
+  </si>
+  <si>
+    <t>11 RA</t>
+  </si>
+  <si>
+    <t>11110</t>
+  </si>
+  <si>
+    <t>00</t>
   </si>
 </sst>
 </file>
@@ -1466,13 +1467,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1493,7 +1494,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1554,6 +1555,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1567,7 +1574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1621,9 +1628,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1639,7 +1652,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1684,9 +1697,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1719,9 +1732,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1927,20 +1940,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV245"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.625" customWidth="1"/>
-    <col min="2" max="4" width="10.625" customWidth="1"/>
-    <col min="5" max="5" width="16.75" customWidth="1"/>
-    <col min="6" max="8" width="10.625" customWidth="1"/>
-    <col min="9" max="9" width="18.875" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:48" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>33</v>
       </c>
@@ -1963,7 +1976,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:48" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:48" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -2021,7 +2034,7 @@
       <c r="AU2" s="4"/>
       <c r="AV2" s="4"/>
     </row>
-    <row r="3" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2087,7 +2100,7 @@
       <c r="AU3" s="4"/>
       <c r="AV3" s="4"/>
     </row>
-    <row r="4" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -2153,7 +2166,7 @@
       <c r="AU4" s="4"/>
       <c r="AV4" s="4"/>
     </row>
-    <row r="5" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2207,7 +2220,7 @@
       <c r="AU5" s="4"/>
       <c r="AV5" s="4"/>
     </row>
-    <row r="6" spans="1:48" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:48" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -2267,7 +2280,7 @@
       <c r="AU6" s="4"/>
       <c r="AV6" s="4"/>
     </row>
-    <row r="7" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2276,7 +2289,7 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>58</v>
@@ -2333,7 +2346,7 @@
       <c r="AU7" s="4"/>
       <c r="AV7" s="4"/>
     </row>
-    <row r="8" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2342,7 +2355,7 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>59</v>
@@ -2399,7 +2412,7 @@
       <c r="AU8" s="4"/>
       <c r="AV8" s="4"/>
     </row>
-    <row r="9" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -2453,7 +2466,7 @@
       <c r="AU9" s="4"/>
       <c r="AV9" s="4"/>
     </row>
-    <row r="10" spans="1:48" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:48" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2507,9 +2520,9 @@
       <c r="AU10" s="4"/>
       <c r="AV10" s="4"/>
     </row>
-    <row r="11" spans="1:48" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:48" s="4" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>69</v>
@@ -2524,7 +2537,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -2541,15 +2554,15 @@
         <v>2</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="13" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>71</v>
@@ -2564,12 +2577,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>72</v>
@@ -2578,13 +2591,13 @@
         <v>63</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="15" spans="1:48" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="15" spans="1:48" s="4" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>38</v>
       </c>
@@ -2598,18 +2611,18 @@
         <v>64</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="16" spans="1:48" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="16" spans="1:48" s="4" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>74</v>
@@ -2618,12 +2631,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>75</v>
@@ -2632,12 +2645,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>76</v>
@@ -2646,12 +2659,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" s="4" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>77</v>
@@ -2660,7 +2673,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" s="4" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>78</v>
       </c>
@@ -2668,74 +2681,74 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" spans="1:5" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="6" t="s">
+    </row>
+    <row r="26" spans="1:5" s="4" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="4" t="s">
-        <v>199</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>201</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D28" s="4" t="s">
         <v>52</v>
       </c>
@@ -2743,7 +2756,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D29" s="4" t="s">
         <v>53</v>
       </c>
@@ -2751,7 +2764,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D30" s="4" t="s">
         <v>37</v>
       </c>
@@ -2759,7 +2772,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D31" s="4" t="s">
         <v>38</v>
       </c>
@@ -2767,15 +2780,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D32" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="33" spans="1:48" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="33" spans="1:48" s="4" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D33" s="4" t="s">
         <v>47</v>
       </c>
@@ -2783,15 +2796,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -2837,12 +2850,12 @@
       <c r="AU34" s="4"/>
       <c r="AV34" s="4"/>
     </row>
-    <row r="35" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>48</v>
@@ -2891,7 +2904,7 @@
       <c r="AU35" s="4"/>
       <c r="AV35" s="4"/>
     </row>
-    <row r="36" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2941,7 +2954,7 @@
       <c r="AU36" s="4"/>
       <c r="AV36" s="4"/>
     </row>
-    <row r="37" spans="1:48" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:48" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -2989,7 +3002,7 @@
       <c r="AU37" s="4"/>
       <c r="AV37" s="4"/>
     </row>
-    <row r="38" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -3037,7 +3050,7 @@
       <c r="AU38" s="4"/>
       <c r="AV38" s="4"/>
     </row>
-    <row r="39" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -3085,7 +3098,7 @@
       <c r="AU39" s="4"/>
       <c r="AV39" s="4"/>
     </row>
-    <row r="40" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -3133,7 +3146,7 @@
       <c r="AU40" s="4"/>
       <c r="AV40" s="4"/>
     </row>
-    <row r="41" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -3181,7 +3194,7 @@
       <c r="AU41" s="4"/>
       <c r="AV41" s="4"/>
     </row>
-    <row r="42" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -3231,7 +3244,7 @@
       <c r="AU42" s="4"/>
       <c r="AV42" s="4"/>
     </row>
-    <row r="43" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -3281,7 +3294,7 @@
       <c r="AU43" s="4"/>
       <c r="AV43" s="4"/>
     </row>
-    <row r="44" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -3331,7 +3344,7 @@
       <c r="AU44" s="4"/>
       <c r="AV44" s="4"/>
     </row>
-    <row r="45" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -3381,7 +3394,7 @@
       <c r="AU45" s="4"/>
       <c r="AV45" s="4"/>
     </row>
-    <row r="46" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3431,7 +3444,7 @@
       <c r="AU46" s="1"/>
       <c r="AV46" s="1"/>
     </row>
-    <row r="47" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3481,7 +3494,7 @@
       <c r="AU47" s="1"/>
       <c r="AV47" s="1"/>
     </row>
-    <row r="48" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3531,7 +3544,7 @@
       <c r="AU48" s="1"/>
       <c r="AV48" s="1"/>
     </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3581,7 +3594,7 @@
       <c r="AU49" s="1"/>
       <c r="AV49" s="1"/>
     </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3631,7 +3644,7 @@
       <c r="AU50" s="1"/>
       <c r="AV50" s="1"/>
     </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3681,7 +3694,7 @@
       <c r="AU51" s="1"/>
       <c r="AV51" s="1"/>
     </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3731,7 +3744,7 @@
       <c r="AU52" s="1"/>
       <c r="AV52" s="1"/>
     </row>
-    <row r="53" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3781,7 +3794,7 @@
       <c r="AU53" s="1"/>
       <c r="AV53" s="1"/>
     </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3831,7 +3844,7 @@
       <c r="AU54" s="1"/>
       <c r="AV54" s="1"/>
     </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3881,7 +3894,7 @@
       <c r="AU55" s="1"/>
       <c r="AV55" s="1"/>
     </row>
-    <row r="56" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3931,7 +3944,7 @@
       <c r="AU56" s="1"/>
       <c r="AV56" s="1"/>
     </row>
-    <row r="57" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3981,7 +3994,7 @@
       <c r="AU57" s="1"/>
       <c r="AV57" s="1"/>
     </row>
-    <row r="58" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -4031,7 +4044,7 @@
       <c r="AU58" s="1"/>
       <c r="AV58" s="1"/>
     </row>
-    <row r="59" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -4081,7 +4094,7 @@
       <c r="AU59" s="1"/>
       <c r="AV59" s="1"/>
     </row>
-    <row r="60" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -4131,7 +4144,7 @@
       <c r="AU60" s="1"/>
       <c r="AV60" s="1"/>
     </row>
-    <row r="61" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -4181,7 +4194,7 @@
       <c r="AU61" s="1"/>
       <c r="AV61" s="1"/>
     </row>
-    <row r="62" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -4231,7 +4244,7 @@
       <c r="AU62" s="1"/>
       <c r="AV62" s="1"/>
     </row>
-    <row r="63" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -4281,7 +4294,7 @@
       <c r="AU63" s="1"/>
       <c r="AV63" s="1"/>
     </row>
-    <row r="64" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -4331,7 +4344,7 @@
       <c r="AU64" s="1"/>
       <c r="AV64" s="1"/>
     </row>
-    <row r="65" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -4381,7 +4394,7 @@
       <c r="AU65" s="1"/>
       <c r="AV65" s="1"/>
     </row>
-    <row r="66" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4431,7 +4444,7 @@
       <c r="AU66" s="1"/>
       <c r="AV66" s="1"/>
     </row>
-    <row r="67" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4481,7 +4494,7 @@
       <c r="AU67" s="1"/>
       <c r="AV67" s="1"/>
     </row>
-    <row r="68" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -4531,7 +4544,7 @@
       <c r="AU68" s="1"/>
       <c r="AV68" s="1"/>
     </row>
-    <row r="69" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -4581,7 +4594,7 @@
       <c r="AU69" s="1"/>
       <c r="AV69" s="1"/>
     </row>
-    <row r="70" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -4631,7 +4644,7 @@
       <c r="AU70" s="1"/>
       <c r="AV70" s="1"/>
     </row>
-    <row r="71" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -4681,7 +4694,7 @@
       <c r="AU71" s="1"/>
       <c r="AV71" s="1"/>
     </row>
-    <row r="72" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -4731,7 +4744,7 @@
       <c r="AU72" s="1"/>
       <c r="AV72" s="1"/>
     </row>
-    <row r="73" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -4781,7 +4794,7 @@
       <c r="AU73" s="1"/>
       <c r="AV73" s="1"/>
     </row>
-    <row r="74" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4831,7 +4844,7 @@
       <c r="AU74" s="1"/>
       <c r="AV74" s="1"/>
     </row>
-    <row r="75" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -4881,7 +4894,7 @@
       <c r="AU75" s="1"/>
       <c r="AV75" s="1"/>
     </row>
-    <row r="76" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -4931,7 +4944,7 @@
       <c r="AU76" s="1"/>
       <c r="AV76" s="1"/>
     </row>
-    <row r="77" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -4981,7 +4994,7 @@
       <c r="AU77" s="1"/>
       <c r="AV77" s="1"/>
     </row>
-    <row r="78" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -5031,7 +5044,7 @@
       <c r="AU78" s="1"/>
       <c r="AV78" s="1"/>
     </row>
-    <row r="79" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -5081,7 +5094,7 @@
       <c r="AU79" s="1"/>
       <c r="AV79" s="1"/>
     </row>
-    <row r="80" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -5131,7 +5144,7 @@
       <c r="AU80" s="1"/>
       <c r="AV80" s="1"/>
     </row>
-    <row r="81" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -5181,7 +5194,7 @@
       <c r="AU81" s="1"/>
       <c r="AV81" s="1"/>
     </row>
-    <row r="82" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -5231,7 +5244,7 @@
       <c r="AU82" s="1"/>
       <c r="AV82" s="1"/>
     </row>
-    <row r="83" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -5281,7 +5294,7 @@
       <c r="AU83" s="1"/>
       <c r="AV83" s="1"/>
     </row>
-    <row r="84" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -5331,7 +5344,7 @@
       <c r="AU84" s="1"/>
       <c r="AV84" s="1"/>
     </row>
-    <row r="85" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -5381,7 +5394,7 @@
       <c r="AU85" s="1"/>
       <c r="AV85" s="1"/>
     </row>
-    <row r="86" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -5431,7 +5444,7 @@
       <c r="AU86" s="1"/>
       <c r="AV86" s="1"/>
     </row>
-    <row r="87" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -5481,7 +5494,7 @@
       <c r="AU87" s="1"/>
       <c r="AV87" s="1"/>
     </row>
-    <row r="88" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -5531,7 +5544,7 @@
       <c r="AU88" s="1"/>
       <c r="AV88" s="1"/>
     </row>
-    <row r="89" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -5581,7 +5594,7 @@
       <c r="AU89" s="1"/>
       <c r="AV89" s="1"/>
     </row>
-    <row r="90" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -5631,7 +5644,7 @@
       <c r="AU90" s="1"/>
       <c r="AV90" s="1"/>
     </row>
-    <row r="91" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -5681,7 +5694,7 @@
       <c r="AU91" s="1"/>
       <c r="AV91" s="1"/>
     </row>
-    <row r="92" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -5731,7 +5744,7 @@
       <c r="AU92" s="1"/>
       <c r="AV92" s="1"/>
     </row>
-    <row r="93" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -5781,7 +5794,7 @@
       <c r="AU93" s="1"/>
       <c r="AV93" s="1"/>
     </row>
-    <row r="94" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -5831,7 +5844,7 @@
       <c r="AU94" s="1"/>
       <c r="AV94" s="1"/>
     </row>
-    <row r="95" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -5881,7 +5894,7 @@
       <c r="AU95" s="1"/>
       <c r="AV95" s="1"/>
     </row>
-    <row r="96" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -5931,7 +5944,7 @@
       <c r="AU96" s="1"/>
       <c r="AV96" s="1"/>
     </row>
-    <row r="97" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -5981,7 +5994,7 @@
       <c r="AU97" s="1"/>
       <c r="AV97" s="1"/>
     </row>
-    <row r="98" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -6031,7 +6044,7 @@
       <c r="AU98" s="1"/>
       <c r="AV98" s="1"/>
     </row>
-    <row r="99" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -6081,7 +6094,7 @@
       <c r="AU99" s="1"/>
       <c r="AV99" s="1"/>
     </row>
-    <row r="100" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -6131,7 +6144,7 @@
       <c r="AU100" s="1"/>
       <c r="AV100" s="1"/>
     </row>
-    <row r="101" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -6181,7 +6194,7 @@
       <c r="AU101" s="1"/>
       <c r="AV101" s="1"/>
     </row>
-    <row r="102" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -6231,7 +6244,7 @@
       <c r="AU102" s="1"/>
       <c r="AV102" s="1"/>
     </row>
-    <row r="103" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -6281,7 +6294,7 @@
       <c r="AU103" s="1"/>
       <c r="AV103" s="1"/>
     </row>
-    <row r="104" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -6331,7 +6344,7 @@
       <c r="AU104" s="1"/>
       <c r="AV104" s="1"/>
     </row>
-    <row r="105" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -6381,7 +6394,7 @@
       <c r="AU105" s="1"/>
       <c r="AV105" s="1"/>
     </row>
-    <row r="106" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -6431,7 +6444,7 @@
       <c r="AU106" s="1"/>
       <c r="AV106" s="1"/>
     </row>
-    <row r="107" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -6481,7 +6494,7 @@
       <c r="AU107" s="1"/>
       <c r="AV107" s="1"/>
     </row>
-    <row r="108" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -6531,7 +6544,7 @@
       <c r="AU108" s="1"/>
       <c r="AV108" s="1"/>
     </row>
-    <row r="109" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -6581,7 +6594,7 @@
       <c r="AU109" s="1"/>
       <c r="AV109" s="1"/>
     </row>
-    <row r="110" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -6631,7 +6644,7 @@
       <c r="AU110" s="1"/>
       <c r="AV110" s="1"/>
     </row>
-    <row r="111" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -6681,7 +6694,7 @@
       <c r="AU111" s="1"/>
       <c r="AV111" s="1"/>
     </row>
-    <row r="112" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -6731,7 +6744,7 @@
       <c r="AU112" s="1"/>
       <c r="AV112" s="1"/>
     </row>
-    <row r="113" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -6781,7 +6794,7 @@
       <c r="AU113" s="1"/>
       <c r="AV113" s="1"/>
     </row>
-    <row r="114" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -6831,7 +6844,7 @@
       <c r="AU114" s="1"/>
       <c r="AV114" s="1"/>
     </row>
-    <row r="115" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -6881,7 +6894,7 @@
       <c r="AU115" s="1"/>
       <c r="AV115" s="1"/>
     </row>
-    <row r="116" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -6931,7 +6944,7 @@
       <c r="AU116" s="1"/>
       <c r="AV116" s="1"/>
     </row>
-    <row r="117" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -6981,7 +6994,7 @@
       <c r="AU117" s="1"/>
       <c r="AV117" s="1"/>
     </row>
-    <row r="118" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -7031,7 +7044,7 @@
       <c r="AU118" s="1"/>
       <c r="AV118" s="1"/>
     </row>
-    <row r="119" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -7081,7 +7094,7 @@
       <c r="AU119" s="1"/>
       <c r="AV119" s="1"/>
     </row>
-    <row r="120" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -7131,7 +7144,7 @@
       <c r="AU120" s="1"/>
       <c r="AV120" s="1"/>
     </row>
-    <row r="121" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -7181,7 +7194,7 @@
       <c r="AU121" s="1"/>
       <c r="AV121" s="1"/>
     </row>
-    <row r="122" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -7231,7 +7244,7 @@
       <c r="AU122" s="1"/>
       <c r="AV122" s="1"/>
     </row>
-    <row r="123" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -7281,7 +7294,7 @@
       <c r="AU123" s="1"/>
       <c r="AV123" s="1"/>
     </row>
-    <row r="124" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -7331,7 +7344,7 @@
       <c r="AU124" s="1"/>
       <c r="AV124" s="1"/>
     </row>
-    <row r="125" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -7381,7 +7394,7 @@
       <c r="AU125" s="1"/>
       <c r="AV125" s="1"/>
     </row>
-    <row r="126" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -7431,7 +7444,7 @@
       <c r="AU126" s="1"/>
       <c r="AV126" s="1"/>
     </row>
-    <row r="127" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -7481,7 +7494,7 @@
       <c r="AU127" s="1"/>
       <c r="AV127" s="1"/>
     </row>
-    <row r="128" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -7531,7 +7544,7 @@
       <c r="AU128" s="1"/>
       <c r="AV128" s="1"/>
     </row>
-    <row r="129" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -7581,7 +7594,7 @@
       <c r="AU129" s="1"/>
       <c r="AV129" s="1"/>
     </row>
-    <row r="130" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -7631,7 +7644,7 @@
       <c r="AU130" s="1"/>
       <c r="AV130" s="1"/>
     </row>
-    <row r="131" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -7681,7 +7694,7 @@
       <c r="AU131" s="1"/>
       <c r="AV131" s="1"/>
     </row>
-    <row r="132" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -7731,7 +7744,7 @@
       <c r="AU132" s="1"/>
       <c r="AV132" s="1"/>
     </row>
-    <row r="133" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -7781,7 +7794,7 @@
       <c r="AU133" s="1"/>
       <c r="AV133" s="1"/>
     </row>
-    <row r="134" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -7831,7 +7844,7 @@
       <c r="AU134" s="1"/>
       <c r="AV134" s="1"/>
     </row>
-    <row r="135" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -7881,7 +7894,7 @@
       <c r="AU135" s="1"/>
       <c r="AV135" s="1"/>
     </row>
-    <row r="136" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -7931,7 +7944,7 @@
       <c r="AU136" s="1"/>
       <c r="AV136" s="1"/>
     </row>
-    <row r="137" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -7981,7 +7994,7 @@
       <c r="AU137" s="1"/>
       <c r="AV137" s="1"/>
     </row>
-    <row r="138" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -8031,7 +8044,7 @@
       <c r="AU138" s="1"/>
       <c r="AV138" s="1"/>
     </row>
-    <row r="139" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -8081,7 +8094,7 @@
       <c r="AU139" s="1"/>
       <c r="AV139" s="1"/>
     </row>
-    <row r="140" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -8131,7 +8144,7 @@
       <c r="AU140" s="1"/>
       <c r="AV140" s="1"/>
     </row>
-    <row r="141" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -8181,7 +8194,7 @@
       <c r="AU141" s="1"/>
       <c r="AV141" s="1"/>
     </row>
-    <row r="142" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -8231,7 +8244,7 @@
       <c r="AU142" s="1"/>
       <c r="AV142" s="1"/>
     </row>
-    <row r="143" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -8281,7 +8294,7 @@
       <c r="AU143" s="1"/>
       <c r="AV143" s="1"/>
     </row>
-    <row r="144" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -8331,7 +8344,7 @@
       <c r="AU144" s="1"/>
       <c r="AV144" s="1"/>
     </row>
-    <row r="145" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -8381,7 +8394,7 @@
       <c r="AU145" s="1"/>
       <c r="AV145" s="1"/>
     </row>
-    <row r="146" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -8431,7 +8444,7 @@
       <c r="AU146" s="1"/>
       <c r="AV146" s="1"/>
     </row>
-    <row r="147" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -8481,7 +8494,7 @@
       <c r="AU147" s="1"/>
       <c r="AV147" s="1"/>
     </row>
-    <row r="148" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -8531,7 +8544,7 @@
       <c r="AU148" s="1"/>
       <c r="AV148" s="1"/>
     </row>
-    <row r="149" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -8581,7 +8594,7 @@
       <c r="AU149" s="1"/>
       <c r="AV149" s="1"/>
     </row>
-    <row r="150" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -8631,7 +8644,7 @@
       <c r="AU150" s="1"/>
       <c r="AV150" s="1"/>
     </row>
-    <row r="151" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -8681,7 +8694,7 @@
       <c r="AU151" s="1"/>
       <c r="AV151" s="1"/>
     </row>
-    <row r="152" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -8731,7 +8744,7 @@
       <c r="AU152" s="1"/>
       <c r="AV152" s="1"/>
     </row>
-    <row r="153" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -8781,7 +8794,7 @@
       <c r="AU153" s="1"/>
       <c r="AV153" s="1"/>
     </row>
-    <row r="154" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -8831,7 +8844,7 @@
       <c r="AU154" s="1"/>
       <c r="AV154" s="1"/>
     </row>
-    <row r="155" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -8881,7 +8894,7 @@
       <c r="AU155" s="1"/>
       <c r="AV155" s="1"/>
     </row>
-    <row r="156" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -8931,7 +8944,7 @@
       <c r="AU156" s="1"/>
       <c r="AV156" s="1"/>
     </row>
-    <row r="157" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -8981,7 +8994,7 @@
       <c r="AU157" s="1"/>
       <c r="AV157" s="1"/>
     </row>
-    <row r="158" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -9031,7 +9044,7 @@
       <c r="AU158" s="1"/>
       <c r="AV158" s="1"/>
     </row>
-    <row r="159" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -9081,7 +9094,7 @@
       <c r="AU159" s="1"/>
       <c r="AV159" s="1"/>
     </row>
-    <row r="160" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -9131,7 +9144,7 @@
       <c r="AU160" s="1"/>
       <c r="AV160" s="1"/>
     </row>
-    <row r="161" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -9181,7 +9194,7 @@
       <c r="AU161" s="1"/>
       <c r="AV161" s="1"/>
     </row>
-    <row r="162" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -9231,7 +9244,7 @@
       <c r="AU162" s="1"/>
       <c r="AV162" s="1"/>
     </row>
-    <row r="163" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -9281,7 +9294,7 @@
       <c r="AU163" s="1"/>
       <c r="AV163" s="1"/>
     </row>
-    <row r="164" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -9331,7 +9344,7 @@
       <c r="AU164" s="1"/>
       <c r="AV164" s="1"/>
     </row>
-    <row r="165" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -9381,7 +9394,7 @@
       <c r="AU165" s="1"/>
       <c r="AV165" s="1"/>
     </row>
-    <row r="166" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -9431,7 +9444,7 @@
       <c r="AU166" s="1"/>
       <c r="AV166" s="1"/>
     </row>
-    <row r="167" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -9481,7 +9494,7 @@
       <c r="AU167" s="1"/>
       <c r="AV167" s="1"/>
     </row>
-    <row r="168" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -9531,7 +9544,7 @@
       <c r="AU168" s="1"/>
       <c r="AV168" s="1"/>
     </row>
-    <row r="169" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -9581,7 +9594,7 @@
       <c r="AU169" s="1"/>
       <c r="AV169" s="1"/>
     </row>
-    <row r="170" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -9631,7 +9644,7 @@
       <c r="AU170" s="1"/>
       <c r="AV170" s="1"/>
     </row>
-    <row r="171" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -9681,7 +9694,7 @@
       <c r="AU171" s="1"/>
       <c r="AV171" s="1"/>
     </row>
-    <row r="172" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -9731,7 +9744,7 @@
       <c r="AU172" s="1"/>
       <c r="AV172" s="1"/>
     </row>
-    <row r="173" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -9781,7 +9794,7 @@
       <c r="AU173" s="1"/>
       <c r="AV173" s="1"/>
     </row>
-    <row r="174" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -9831,7 +9844,7 @@
       <c r="AU174" s="1"/>
       <c r="AV174" s="1"/>
     </row>
-    <row r="175" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -9881,7 +9894,7 @@
       <c r="AU175" s="1"/>
       <c r="AV175" s="1"/>
     </row>
-    <row r="176" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -9931,7 +9944,7 @@
       <c r="AU176" s="1"/>
       <c r="AV176" s="1"/>
     </row>
-    <row r="177" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -9981,7 +9994,7 @@
       <c r="AU177" s="1"/>
       <c r="AV177" s="1"/>
     </row>
-    <row r="178" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -10031,7 +10044,7 @@
       <c r="AU178" s="1"/>
       <c r="AV178" s="1"/>
     </row>
-    <row r="179" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -10081,7 +10094,7 @@
       <c r="AU179" s="1"/>
       <c r="AV179" s="1"/>
     </row>
-    <row r="180" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -10131,7 +10144,7 @@
       <c r="AU180" s="1"/>
       <c r="AV180" s="1"/>
     </row>
-    <row r="181" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -10181,7 +10194,7 @@
       <c r="AU181" s="1"/>
       <c r="AV181" s="1"/>
     </row>
-    <row r="182" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -10231,7 +10244,7 @@
       <c r="AU182" s="1"/>
       <c r="AV182" s="1"/>
     </row>
-    <row r="183" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -10281,7 +10294,7 @@
       <c r="AU183" s="1"/>
       <c r="AV183" s="1"/>
     </row>
-    <row r="184" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -10331,7 +10344,7 @@
       <c r="AU184" s="1"/>
       <c r="AV184" s="1"/>
     </row>
-    <row r="185" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -10381,7 +10394,7 @@
       <c r="AU185" s="1"/>
       <c r="AV185" s="1"/>
     </row>
-    <row r="186" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -10431,7 +10444,7 @@
       <c r="AU186" s="1"/>
       <c r="AV186" s="1"/>
     </row>
-    <row r="187" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -10481,7 +10494,7 @@
       <c r="AU187" s="1"/>
       <c r="AV187" s="1"/>
     </row>
-    <row r="188" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -10531,7 +10544,7 @@
       <c r="AU188" s="1"/>
       <c r="AV188" s="1"/>
     </row>
-    <row r="189" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -10581,7 +10594,7 @@
       <c r="AU189" s="1"/>
       <c r="AV189" s="1"/>
     </row>
-    <row r="190" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -10631,7 +10644,7 @@
       <c r="AU190" s="1"/>
       <c r="AV190" s="1"/>
     </row>
-    <row r="191" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -10681,7 +10694,7 @@
       <c r="AU191" s="1"/>
       <c r="AV191" s="1"/>
     </row>
-    <row r="192" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -10731,7 +10744,7 @@
       <c r="AU192" s="1"/>
       <c r="AV192" s="1"/>
     </row>
-    <row r="193" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -10781,7 +10794,7 @@
       <c r="AU193" s="1"/>
       <c r="AV193" s="1"/>
     </row>
-    <row r="194" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -10831,7 +10844,7 @@
       <c r="AU194" s="1"/>
       <c r="AV194" s="1"/>
     </row>
-    <row r="195" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -10881,7 +10894,7 @@
       <c r="AU195" s="1"/>
       <c r="AV195" s="1"/>
     </row>
-    <row r="196" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -10931,7 +10944,7 @@
       <c r="AU196" s="1"/>
       <c r="AV196" s="1"/>
     </row>
-    <row r="197" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -10981,7 +10994,7 @@
       <c r="AU197" s="1"/>
       <c r="AV197" s="1"/>
     </row>
-    <row r="198" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -11031,7 +11044,7 @@
       <c r="AU198" s="1"/>
       <c r="AV198" s="1"/>
     </row>
-    <row r="199" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -11081,7 +11094,7 @@
       <c r="AU199" s="1"/>
       <c r="AV199" s="1"/>
     </row>
-    <row r="200" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -11131,7 +11144,7 @@
       <c r="AU200" s="1"/>
       <c r="AV200" s="1"/>
     </row>
-    <row r="201" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -11181,7 +11194,7 @@
       <c r="AU201" s="1"/>
       <c r="AV201" s="1"/>
     </row>
-    <row r="202" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -11231,7 +11244,7 @@
       <c r="AU202" s="1"/>
       <c r="AV202" s="1"/>
     </row>
-    <row r="203" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -11281,7 +11294,7 @@
       <c r="AU203" s="1"/>
       <c r="AV203" s="1"/>
     </row>
-    <row r="204" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -11331,7 +11344,7 @@
       <c r="AU204" s="1"/>
       <c r="AV204" s="1"/>
     </row>
-    <row r="205" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -11381,7 +11394,7 @@
       <c r="AU205" s="1"/>
       <c r="AV205" s="1"/>
     </row>
-    <row r="206" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -11431,7 +11444,7 @@
       <c r="AU206" s="1"/>
       <c r="AV206" s="1"/>
     </row>
-    <row r="207" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -11481,7 +11494,7 @@
       <c r="AU207" s="1"/>
       <c r="AV207" s="1"/>
     </row>
-    <row r="208" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -11531,7 +11544,7 @@
       <c r="AU208" s="1"/>
       <c r="AV208" s="1"/>
     </row>
-    <row r="209" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -11581,7 +11594,7 @@
       <c r="AU209" s="1"/>
       <c r="AV209" s="1"/>
     </row>
-    <row r="210" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -11631,7 +11644,7 @@
       <c r="AU210" s="1"/>
       <c r="AV210" s="1"/>
     </row>
-    <row r="211" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -11681,7 +11694,7 @@
       <c r="AU211" s="1"/>
       <c r="AV211" s="1"/>
     </row>
-    <row r="212" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -11731,7 +11744,7 @@
       <c r="AU212" s="1"/>
       <c r="AV212" s="1"/>
     </row>
-    <row r="213" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -11781,7 +11794,7 @@
       <c r="AU213" s="1"/>
       <c r="AV213" s="1"/>
     </row>
-    <row r="214" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -11831,7 +11844,7 @@
       <c r="AU214" s="1"/>
       <c r="AV214" s="1"/>
     </row>
-    <row r="215" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -11881,7 +11894,7 @@
       <c r="AU215" s="1"/>
       <c r="AV215" s="1"/>
     </row>
-    <row r="216" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -11931,7 +11944,7 @@
       <c r="AU216" s="1"/>
       <c r="AV216" s="1"/>
     </row>
-    <row r="217" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
@@ -11981,7 +11994,7 @@
       <c r="AU217" s="1"/>
       <c r="AV217" s="1"/>
     </row>
-    <row r="218" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -12031,7 +12044,7 @@
       <c r="AU218" s="1"/>
       <c r="AV218" s="1"/>
     </row>
-    <row r="219" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
@@ -12081,7 +12094,7 @@
       <c r="AU219" s="1"/>
       <c r="AV219" s="1"/>
     </row>
-    <row r="220" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
@@ -12131,7 +12144,7 @@
       <c r="AU220" s="1"/>
       <c r="AV220" s="1"/>
     </row>
-    <row r="221" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -12181,7 +12194,7 @@
       <c r="AU221" s="1"/>
       <c r="AV221" s="1"/>
     </row>
-    <row r="222" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -12231,7 +12244,7 @@
       <c r="AU222" s="1"/>
       <c r="AV222" s="1"/>
     </row>
-    <row r="223" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -12281,7 +12294,7 @@
       <c r="AU223" s="1"/>
       <c r="AV223" s="1"/>
     </row>
-    <row r="224" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -12331,7 +12344,7 @@
       <c r="AU224" s="1"/>
       <c r="AV224" s="1"/>
     </row>
-    <row r="225" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
@@ -12381,7 +12394,7 @@
       <c r="AU225" s="1"/>
       <c r="AV225" s="1"/>
     </row>
-    <row r="226" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
@@ -12431,7 +12444,7 @@
       <c r="AU226" s="1"/>
       <c r="AV226" s="1"/>
     </row>
-    <row r="227" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
@@ -12481,7 +12494,7 @@
       <c r="AU227" s="1"/>
       <c r="AV227" s="1"/>
     </row>
-    <row r="228" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -12531,7 +12544,7 @@
       <c r="AU228" s="1"/>
       <c r="AV228" s="1"/>
     </row>
-    <row r="229" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
@@ -12581,7 +12594,7 @@
       <c r="AU229" s="1"/>
       <c r="AV229" s="1"/>
     </row>
-    <row r="230" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A230" s="1"/>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
@@ -12631,7 +12644,7 @@
       <c r="AU230" s="1"/>
       <c r="AV230" s="1"/>
     </row>
-    <row r="231" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A231" s="1"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
@@ -12681,7 +12694,7 @@
       <c r="AU231" s="1"/>
       <c r="AV231" s="1"/>
     </row>
-    <row r="232" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A232" s="1"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
@@ -12731,7 +12744,7 @@
       <c r="AU232" s="1"/>
       <c r="AV232" s="1"/>
     </row>
-    <row r="233" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
@@ -12781,7 +12794,7 @@
       <c r="AU233" s="1"/>
       <c r="AV233" s="1"/>
     </row>
-    <row r="234" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A234" s="1"/>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
@@ -12831,7 +12844,7 @@
       <c r="AU234" s="1"/>
       <c r="AV234" s="1"/>
     </row>
-    <row r="235" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A235" s="1"/>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
@@ -12881,7 +12894,7 @@
       <c r="AU235" s="1"/>
       <c r="AV235" s="1"/>
     </row>
-    <row r="236" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A236" s="1"/>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
@@ -12931,7 +12944,7 @@
       <c r="AU236" s="1"/>
       <c r="AV236" s="1"/>
     </row>
-    <row r="237" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A237" s="1"/>
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
@@ -12981,7 +12994,7 @@
       <c r="AU237" s="1"/>
       <c r="AV237" s="1"/>
     </row>
-    <row r="238" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A238" s="1"/>
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
@@ -13031,7 +13044,7 @@
       <c r="AU238" s="1"/>
       <c r="AV238" s="1"/>
     </row>
-    <row r="239" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A239" s="1"/>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
@@ -13081,7 +13094,7 @@
       <c r="AU239" s="1"/>
       <c r="AV239" s="1"/>
     </row>
-    <row r="240" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A240" s="1"/>
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
@@ -13131,7 +13144,7 @@
       <c r="AU240" s="1"/>
       <c r="AV240" s="1"/>
     </row>
-    <row r="241" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A241" s="1"/>
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
@@ -13181,7 +13194,7 @@
       <c r="AU241" s="1"/>
       <c r="AV241" s="1"/>
     </row>
-    <row r="242" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A242" s="1"/>
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
@@ -13231,7 +13244,7 @@
       <c r="AU242" s="1"/>
       <c r="AV242" s="1"/>
     </row>
-    <row r="243" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A243" s="1"/>
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
@@ -13281,7 +13294,7 @@
       <c r="AU243" s="1"/>
       <c r="AV243" s="1"/>
     </row>
-    <row r="244" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A244" s="1"/>
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
@@ -13331,7 +13344,7 @@
       <c r="AU244" s="1"/>
       <c r="AV244" s="1"/>
     </row>
-    <row r="245" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A245" s="1"/>
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
@@ -13399,24 +13412,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="12.625" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="12.625" customWidth="1"/>
-    <col min="6" max="6" width="15.625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="17" width="12.625" customWidth="1"/>
+    <col min="9" max="17" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>84</v>
       </c>
@@ -13430,43 +13443,43 @@
         <v>88</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="H1" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="G1" s="17" t="s">
-        <v>298</v>
-      </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="I1" s="17" t="s">
-        <v>217</v>
-      </c>
       <c r="J1" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="K1" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="L1" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="O1" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="P1" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="P1" s="17" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>89</v>
       </c>
@@ -13480,16 +13493,16 @@
         <v>96</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>228</v>
       </c>
       <c r="I2" s="3">
         <v>0</v>
@@ -13498,27 +13511,27 @@
         <v>0</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q2" s="7"/>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>90</v>
       </c>
@@ -13536,13 +13549,13 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="8" t="s">
-        <v>303</v>
+        <v>318</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -13550,21 +13563,21 @@
         <v>52</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>91</v>
       </c>
@@ -13581,16 +13594,16 @@
         <v>100</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -13598,21 +13611,21 @@
         <v>52</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Q4" s="7"/>
       <c r="R4" s="3"/>
     </row>
-    <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>92</v>
       </c>
@@ -13629,16 +13642,16 @@
         <v>100</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>304</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -13646,29 +13659,29 @@
         <v>52</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q5" s="7"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>106</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>102</v>
@@ -13676,17 +13689,17 @@
       <c r="E6" s="2">
         <v>100</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>305</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -13694,21 +13707,21 @@
         <v>52</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q6" s="7"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>107</v>
       </c>
@@ -13725,19 +13738,19 @@
         <v>52</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>70</v>
@@ -13746,21 +13759,21 @@
         <v>38</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>52</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>108</v>
       </c>
@@ -13774,22 +13787,22 @@
         <v>113</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>71</v>
@@ -13798,21 +13811,21 @@
         <v>38</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Q8" s="7"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>114</v>
       </c>
@@ -13829,42 +13842,42 @@
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>72</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q9" s="7"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>115</v>
       </c>
@@ -13881,42 +13894,42 @@
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q10" s="7"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>100</v>
       </c>
@@ -13933,42 +13946,42 @@
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q11" s="7"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>116</v>
       </c>
@@ -13985,42 +13998,42 @@
         <v>0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>73</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q12" s="7"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>117</v>
       </c>
@@ -14037,17 +14050,17 @@
         <v>38</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>75</v>
@@ -14056,21 +14069,21 @@
         <v>40</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q13" s="7"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>118</v>
       </c>
@@ -14087,42 +14100,42 @@
         <v>52</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>46</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q14" s="7"/>
       <c r="R14" s="3"/>
     </row>
-    <row r="15" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>119</v>
       </c>
@@ -14136,43 +14149,43 @@
         <v>131</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q15" s="7"/>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>120</v>
       </c>
@@ -14186,22 +14199,22 @@
         <v>113</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>277</v>
-      </c>
       <c r="I16" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>76</v>
@@ -14210,29 +14223,29 @@
         <v>37</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q16" s="7"/>
       <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>134</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>138</v>
+        <v>317</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>113</v>
@@ -14240,47 +14253,47 @@
       <c r="E17" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>278</v>
+      <c r="F17" s="19" t="s">
+        <v>277</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="Q17" s="7"/>
       <c r="R17" s="3"/>
     </row>
-    <row r="18" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>135</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>113</v>
@@ -14288,28 +14301,26 @@
       <c r="E18" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>302</v>
-      </c>
+      <c r="F18" s="20"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>0</v>
@@ -14320,15 +14331,15 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="3"/>
     </row>
-    <row r="19" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>136</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>113</v>
@@ -14337,46 +14348,46 @@
         <v>0</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="Q19" s="7"/>
       <c r="R19" s="3"/>
     </row>
-    <row r="20" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>137</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>113</v>
@@ -14385,14 +14396,14 @@
         <v>0</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3" t="s">
@@ -14402,10 +14413,10 @@
         <v>47</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O20" s="3" t="s">
         <v>0</v>
@@ -14416,262 +14427,262 @@
       <c r="Q20" s="7"/>
       <c r="R20" s="3"/>
     </row>
-    <row r="21" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>37</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O21" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q21" s="7"/>
       <c r="R21" s="3"/>
     </row>
-    <row r="22" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>70</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O22" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q22" s="7"/>
       <c r="R22" s="3"/>
     </row>
-    <row r="23" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q23" s="7"/>
       <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O24" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q24" s="7"/>
       <c r="R24" s="3"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>286</v>
+      <c r="F25" s="19" t="s">
+        <v>285</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>70</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O25" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q25" s="7"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>113</v>
@@ -14680,48 +14691,48 @@
         <v>102</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>46</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O26" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q26" s="7"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>113</v>
@@ -14735,41 +14746,41 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>273</v>
-      </c>
       <c r="K27" s="3" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O27" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q27" s="7"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>113</v>
@@ -14778,98 +14789,98 @@
         <v>98</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>288</v>
+        <v>179</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>287</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>70</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O28" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q28" s="7"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>103</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>290</v>
+        <v>211</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>316</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>70</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q29" s="7"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>113</v>
@@ -14880,63 +14891,63 @@
       <c r="E30" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>285</v>
+      <c r="F30" s="19" t="s">
+        <v>284</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>70</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q30" s="7"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>101</v>
       </c>
       <c r="C31" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>169</v>
-      </c>
       <c r="E31" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3" t="s">
@@ -14944,21 +14955,21 @@
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O31" s="3" t="s">
         <v>0</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q31" s="7"/>
       <c r="R31" s="3"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -14973,7 +14984,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="6:18" x14ac:dyDescent="0.15">
+    <row r="33" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -14988,7 +14999,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="6:18" x14ac:dyDescent="0.15">
+    <row r="34" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -15003,7 +15014,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="6:18" x14ac:dyDescent="0.15">
+    <row r="35" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -15018,7 +15029,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="6:18" x14ac:dyDescent="0.15">
+    <row r="36" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -15033,7 +15044,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="6:18" x14ac:dyDescent="0.15">
+    <row r="37" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>

</xml_diff>